<commit_message>
feat: (probably) implement context saver
</commit_message>
<xml_diff>
--- a/mocks/utilities_mvp_mock_format.xlsx
+++ b/mocks/utilities_mvp_mock_format.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Milestone</t>
   </si>
   <si>
-    <t xml:space="preserve">Total, hr. = 300</t>
+    <t xml:space="preserve">Total, hr.</t>
   </si>
   <si>
     <t xml:space="preserve">Front view, hr.</t>
@@ -713,13 +713,14 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A105" activeCellId="0" sqref="A105"/>
+      <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>